<commit_message>
Inserindo informações na tabela
</commit_message>
<xml_diff>
--- a/TabelasCadastroDeFilme.xlsx
+++ b/TabelasCadastroDeFilme.xlsx
@@ -195,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +205,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,32 +248,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,250 +564,250 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <v>0.125</v>
       </c>
-      <c r="D2" s="7">
-        <v>2020</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="11">
+        <v>44124</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="12">
         <v>9.5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="10">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D3" s="7">
-        <v>2021</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="11">
+        <v>44479</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="12">
         <v>8</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D4" s="7">
-        <v>2015</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="11">
+        <v>42129</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="12">
         <v>9</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D5" s="7">
-        <v>2021</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="11">
+        <v>44208</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="12">
         <v>9</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="13">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D6" s="10">
-        <v>1995</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="11">
+        <v>34835</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="12">
         <v>10</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="4" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>